<commit_message>
Modify Excel output by reflection and attribute
</commit_message>
<xml_diff>
--- a/TestExcelOutput/excelTemplate/PDFTemp/検収記録.xlsx
+++ b/TestExcelOutput/excelTemplate/PDFTemp/検収記録.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\4_TestExcelOut\TestExcelOutput\excelTemplate\PDFTemp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D38B7073-6851-4002-BC19-8E37EE034443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8566E4B4-1299-4DCB-83CB-EFA9C5726988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3860" yWindow="1120" windowWidth="14450" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="検収記録_例.店舗全体" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">検収記録_例.店舗全体!$A$1:$K$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">検収記録_例.店舗全体!$A$1:$K$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,14 +31,14 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>承認者</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>20XX年　　4月　XX日</t>
     <rPh sb="12" eb="13">
       <t>ニチ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>検収記録（日報）</t>
@@ -51,14 +51,14 @@
     <rPh sb="5" eb="7">
       <t>ニッポウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>品名</t>
     <rPh sb="0" eb="2">
       <t>ヒンメイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>受入時間</t>
@@ -71,7 +71,7 @@
     <rPh sb="2" eb="4">
       <t>ジカン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>外箱に異常はないか                                                      （包装の破れや液漏れ等）</t>
@@ -93,7 +93,7 @@
     <rPh sb="73" eb="74">
       <t>トウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>品物名や数量等、注文通りに納品されているか</t>
@@ -118,7 +118,7 @@
     <rPh sb="13" eb="15">
       <t>ノウヒン</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>保管温度が守られていたか</t>
@@ -131,7 +131,7 @@
     <rPh sb="5" eb="6">
       <t>マモ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>農産物と水産物の場合　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　：産地と品種/魚類</t>
@@ -153,21 +153,21 @@
     <rPh sb="54" eb="56">
       <t>ギョルイ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>記録者</t>
     <rPh sb="0" eb="3">
       <t>キロクシャ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>備考</t>
     <rPh sb="0" eb="2">
       <t>ビコウ</t>
     </rPh>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>数量</t>
@@ -187,12 +187,20 @@
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
     <numFmt numFmtId="177" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,73 +300,55 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -646,10 +636,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -684,17 +674,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="21"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12">
@@ -708,7 +698,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="21"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" s="6" customFormat="1">
@@ -722,7 +712,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:12" ht="50.15" customHeight="1">
       <c r="A5" s="7" t="s">
@@ -731,19 +721,19 @@
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -775,192 +765,67 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="13"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="14"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="15"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="15"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="15"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="15"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="15"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" s="19" customFormat="1">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="K2:K4"/>
   </mergeCells>
-  <phoneticPr fontId="3"/>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="43" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>